<commit_message>
changes in web pages
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,17 +475,17 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>77.5</v>
+        <v>64</v>
       </c>
       <c r="D2" t="n">
-        <v>72.5</v>
+        <v>60.8</v>
       </c>
       <c r="E2" t="n">
-        <v>75</v>
+        <v>62.4</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>statistics</t>
         </is>
       </c>
     </row>
@@ -495,93 +495,21 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>sairaj pawar.pdf</t>
+          <t>sairj.pdf</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>77.5</v>
+        <v>22</v>
       </c>
       <c r="D3" t="n">
-        <v>72.5</v>
+        <v>24.4</v>
       </c>
       <c r="E3" t="n">
-        <v>75</v>
+        <v>23.2</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Shardul mode.pdf</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>43.75</v>
-      </c>
-      <c r="D4" t="n">
-        <v>43.25</v>
-      </c>
-      <c r="E4" t="n">
-        <v>43.5</v>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>sql, excel</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>sairj.pdf</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>10</v>
-      </c>
-      <c r="D5" t="n">
-        <v>14</v>
-      </c>
-      <c r="E5" t="n">
-        <v>12</v>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>python, sql, excel, data analysis</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>subhash dev.pdf</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>10</v>
-      </c>
-      <c r="D6" t="n">
-        <v>14</v>
-      </c>
-      <c r="E6" t="n">
-        <v>12</v>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>python, sql, excel, data analysis</t>
+          <t>python, statistics, pandas, data analysis</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Added personalized ranking based on the skill
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,17 +471,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>sar.pdf</t>
+          <t>Shardul mode.pdf</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="D2" t="n">
-        <v>60.8</v>
+        <v>66</v>
       </c>
       <c r="E2" t="n">
-        <v>62.4</v>
+        <v>68</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -495,21 +495,93 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>sar.pdf</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>64</v>
+      </c>
+      <c r="D3" t="n">
+        <v>60.8</v>
+      </c>
+      <c r="E3" t="n">
+        <v>62.4</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>statistics</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>sairaj pawar.pdf</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>64</v>
+      </c>
+      <c r="D4" t="n">
+        <v>60.8</v>
+      </c>
+      <c r="E4" t="n">
+        <v>62.4</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>statistics</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
           <t>sairj.pdf</t>
         </is>
       </c>
-      <c r="C3" t="n">
+      <c r="C5" t="n">
         <v>22</v>
       </c>
-      <c r="D3" t="n">
+      <c r="D5" t="n">
         <v>24.4</v>
       </c>
-      <c r="E3" t="n">
+      <c r="E5" t="n">
         <v>23.2</v>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="F5" t="inlineStr">
         <is>
           <t>python, statistics, pandas, data analysis</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>subhash dev.pdf</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>10</v>
+      </c>
+      <c r="D6" t="n">
+        <v>14</v>
+      </c>
+      <c r="E6" t="n">
+        <v>12</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>python, machine learning, statistics, pandas, data analysis</t>
         </is>
       </c>
     </row>

</xml_diff>